<commit_message>
cambia jugador si la diferencia es menor de 0,75
</commit_message>
<xml_diff>
--- a/tu_archivo_excel.xlsx
+++ b/tu_archivo_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\OTRAS_PRUEBAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\ALINEACION-MZ-HOCKEY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6400CC7D-FF9B-480C-A2FD-72C87CB7B186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649DEF0B-5DE6-4DA8-B47D-5BE82EA21922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -681,7 +681,7 @@
   <dimension ref="A1:Y90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>